<commit_message>
Tue Mar 26 06:50:04 AM CST 2024
</commit_message>
<xml_diff>
--- a/lixiao/performance_templ/assess_绩效+软性考核表.xlsx
+++ b/lixiao/performance_templ/assess_绩效+软性考核表.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
   <si>
     <t>绩效考核汇总</t>
   </si>
@@ -57,6 +57,21 @@
   </si>
   <si>
     <t>英文</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
   <si>
     <t>黄礼闯</t>
@@ -767,9 +782,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="36">
     <font>
@@ -850,6 +865,21 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -858,6 +888,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -866,6 +904,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -874,8 +942,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -890,107 +1003,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1066,175 +1081,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1326,11 +1341,48 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1350,54 +1402,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1406,164 +1410,175 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1720,8 +1735,8 @@
   </cellXfs>
   <cellStyles count="56">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 14 2 2" xfId="1"/>
-    <cellStyle name="常规 2 2 2 2" xfId="2"/>
+    <cellStyle name="常规 2 2 2 2" xfId="1"/>
+    <cellStyle name="常规 14 2 2" xfId="2"/>
     <cellStyle name="60% - Accent6" xfId="3" builtinId="52"/>
     <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
     <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
@@ -2072,10 +2087,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2154,7 +2169,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:17">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
@@ -2170,33 +2185,49 @@
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="O6" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="22" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="23" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B7" s="23">
         <v>1</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="38" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H7" s="39"/>
       <c r="I7" s="23" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="J7" s="48" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K7" s="23">
         <v>0.25</v>
@@ -2425,47 +2456,47 @@
     </row>
     <row r="27" spans="4:4">
       <c r="D27" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="4:11">
       <c r="D28" s="24" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E28" s="40" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G28" s="41" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="I28" s="49" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="J28" s="50" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="K28" s="50" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="4:11">
       <c r="D29" s="25" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F29" s="43"/>
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
       <c r="I29" s="51" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="J29" s="26"/>
       <c r="K29" s="52"/>
@@ -2473,25 +2504,25 @@
     <row r="30" spans="4:11">
       <c r="D30" s="26"/>
       <c r="E30" s="44" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F30" s="43"/>
       <c r="G30" s="26"/>
       <c r="H30" s="26"/>
       <c r="I30" s="51" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="J30" s="26"/>
       <c r="K30" s="52"/>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="27" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="28" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B36" s="28"/>
       <c r="C36" s="28"/>
@@ -2500,7 +2531,7 @@
     </row>
     <row r="37" ht="15.75" spans="1:7">
       <c r="A37" s="29" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B37" s="29"/>
       <c r="C37" s="29"/>
@@ -2511,7 +2542,7 @@
     </row>
     <row r="38" ht="15.75" spans="1:7">
       <c r="A38" s="29" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B38" s="29"/>
       <c r="C38" s="29"/>
@@ -2522,7 +2553,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="30" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B39" s="31"/>
       <c r="C39" s="31"/>
@@ -2575,7 +2606,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2619,7 +2650,7 @@
     </row>
     <row r="3" ht="23.25" spans="1:19">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2642,11 +2673,11 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -2657,33 +2688,33 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="11" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" ht="28.5" customHeight="1" spans="1:19">
       <c r="A6" s="4" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2708,16 +2739,16 @@
         <v>0.01</v>
       </c>
       <c r="P6" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="Q6" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="R6" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="S6" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -2745,16 +2776,16 @@
         <v>0.01</v>
       </c>
       <c r="P7" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="Q7" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="R7" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="S7" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -2782,16 +2813,16 @@
         <v>0.01</v>
       </c>
       <c r="P8" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="Q8" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="R8" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="S8" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -2819,22 +2850,22 @@
         <v>0.01</v>
       </c>
       <c r="P9" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="Q9" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="R9" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="S9" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1" spans="1:19">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
@@ -2858,21 +2889,21 @@
         <v>0.01</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="Q10" s="18" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="R10" s="18" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="S10" s="18" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2897,21 +2928,21 @@
         <v>0.05</v>
       </c>
       <c r="P11" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="Q11" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="R11" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="S11" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="9" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -2936,16 +2967,16 @@
         <v>0.95</v>
       </c>
       <c r="P12" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="Q12" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="R12" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="S12" s="18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tue May 28 06:50:05 AM CST 2024
</commit_message>
<xml_diff>
--- a/lixiao/performance_templ/assess_绩效+软性考核表.xlsx
+++ b/lixiao/performance_templ/assess_绩效+软性考核表.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
   <si>
     <t>绩效考核汇总</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>业务类型</t>
+  </si>
+  <si>
+    <t>类型</t>
   </si>
   <si>
     <t>IF</t>
@@ -865,6 +868,127 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -874,71 +998,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -951,65 +1013,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="7"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -1081,13 +1084,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1097,164 +1256,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1315,6 +1318,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1348,11 +1377,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1368,21 +1403,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1404,6 +1424,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1413,176 +1444,174 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="30" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1679,13 +1708,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1693,9 +1725,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1719,6 +1748,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1735,8 +1770,8 @@
   </cellXfs>
   <cellStyles count="56">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2 2 2 2" xfId="1"/>
-    <cellStyle name="常规 14 2 2" xfId="2"/>
+    <cellStyle name="常规 14 2 2" xfId="1"/>
+    <cellStyle name="常规 2 2 2 2" xfId="2"/>
     <cellStyle name="60% - Accent6" xfId="3" builtinId="52"/>
     <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
     <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
@@ -2087,10 +2122,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2098,45 +2133,48 @@
     <col min="2" max="2" width="5.375" customWidth="1"/>
     <col min="3" max="3" width="14.5" customWidth="1"/>
     <col min="4" max="4" width="9.625" customWidth="1"/>
-    <col min="5" max="5" width="9" style="19" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="8" width="29.375" customWidth="1"/>
-    <col min="9" max="9" width="33.5" customWidth="1"/>
-    <col min="10" max="10" width="27.5" customWidth="1"/>
-    <col min="11" max="11" width="11.125"/>
+    <col min="5" max="5" width="9.625" customWidth="1"/>
+    <col min="6" max="6" width="9" style="19" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="9" width="29.375" customWidth="1"/>
+    <col min="10" max="10" width="33.5" customWidth="1"/>
+    <col min="11" max="11" width="27.5" customWidth="1"/>
+    <col min="12" max="12" width="11.125"/>
   </cols>
   <sheetData>
-    <row r="1" ht="33" customHeight="1" spans="1:11">
+    <row r="1" ht="33" customHeight="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="32"/>
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
-    </row>
-    <row r="3" ht="23.25" spans="1:11">
+      <c r="L1" s="20"/>
+    </row>
+    <row r="3" ht="23.25" spans="1:12">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
       <c r="D3" s="21"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="33"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L3" s="21"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="22" t="s">
         <v>2</v>
       </c>
@@ -2152,43 +2190,44 @@
       <c r="E5" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="35"/>
-      <c r="I5" s="22" t="s">
+      <c r="H5" s="36" t="s">
         <v>9</v>
       </c>
+      <c r="I5" s="36"/>
       <c r="J5" s="22" t="s">
         <v>10</v>
       </c>
       <c r="K5" s="22" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="L5" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="36" t="s">
+      <c r="E6" s="37"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="22"/>
+      <c r="I6" s="48" t="s">
+        <v>14</v>
+      </c>
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
       <c r="L6" s="22"/>
-      <c r="M6" s="22" t="s">
-        <v>14</v>
-      </c>
+      <c r="M6" s="22"/>
       <c r="N6" s="22" t="s">
         <v>15</v>
       </c>
@@ -2201,375 +2240,403 @@
       <c r="Q6" s="22" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="R6" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="23">
         <v>1</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="38" t="s">
+      <c r="E7" s="23"/>
+      <c r="F7" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="39"/>
-      <c r="I7" s="23" t="s">
+      <c r="G7" s="23"/>
+      <c r="H7" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="48" t="s">
+      <c r="I7" s="49"/>
+      <c r="J7" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="23">
+      <c r="K7" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="23">
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="38"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="23"/>
       <c r="H8" s="39"/>
-      <c r="I8" s="23"/>
+      <c r="I8" s="49"/>
       <c r="J8" s="23"/>
       <c r="K8" s="23"/>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8" s="23"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="23"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="38"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="23"/>
       <c r="H9" s="39"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="23"/>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="I9" s="49"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="23"/>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="23"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="38"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="23"/>
       <c r="H10" s="39"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="23"/>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="I10" s="49"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="23"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="23"/>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="38"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="23"/>
       <c r="H11" s="39"/>
-      <c r="I11" s="23"/>
+      <c r="I11" s="49"/>
       <c r="J11" s="23"/>
       <c r="K11" s="23"/>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11" s="23"/>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="23"/>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="38"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="23"/>
       <c r="H12" s="39"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="23"/>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="I12" s="49"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="23"/>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="23"/>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="38"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="23"/>
       <c r="H13" s="39"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="23"/>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="I13" s="49"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="23"/>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="23"/>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="38"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="23"/>
       <c r="H14" s="39"/>
-      <c r="I14" s="23"/>
+      <c r="I14" s="49"/>
       <c r="J14" s="23"/>
       <c r="K14" s="23"/>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14" s="23"/>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="23"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="38"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="23"/>
       <c r="H15" s="39"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="23"/>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="I15" s="49"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="23"/>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="23"/>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
       <c r="D16" s="23"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="38"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="23"/>
       <c r="H16" s="39"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="23"/>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="I16" s="49"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="50"/>
+      <c r="L16" s="23"/>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="23"/>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="38"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="23"/>
       <c r="H17" s="39"/>
-      <c r="I17" s="23"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="23"/>
       <c r="K17" s="23"/>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17" s="23"/>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="23"/>
       <c r="B18" s="23"/>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="38"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="23"/>
       <c r="H18" s="39"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="23"/>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="I18" s="49"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="23"/>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="23"/>
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="38"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="23"/>
       <c r="H19" s="39"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="23"/>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="I19" s="49"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="23"/>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="23"/>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="38"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="23"/>
       <c r="H20" s="39"/>
-      <c r="I20" s="23"/>
+      <c r="I20" s="49"/>
       <c r="J20" s="23"/>
       <c r="K20" s="23"/>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20" s="23"/>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="23"/>
       <c r="B21" s="23"/>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="38"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="23"/>
       <c r="H21" s="39"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="23"/>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="I21" s="49"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="23"/>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="23"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="38"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="23"/>
       <c r="H22" s="39"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="48"/>
-      <c r="K22" s="23"/>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="I22" s="49"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="23"/>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="23"/>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
       <c r="D23" s="23"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="38"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="23"/>
       <c r="H23" s="39"/>
-      <c r="I23" s="23"/>
+      <c r="I23" s="49"/>
       <c r="J23" s="23"/>
       <c r="K23" s="23"/>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="L23" s="23"/>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="23"/>
       <c r="B24" s="23"/>
       <c r="C24" s="23"/>
       <c r="D24" s="23"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="38"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="23"/>
       <c r="H24" s="39"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="23"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="23"/>
     </row>
     <row r="27" spans="4:4">
       <c r="D27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="4:11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="4:12">
       <c r="D28" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="24" t="s">
+      <c r="E28" s="24"/>
+      <c r="F28" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="G28" s="41" t="s">
+      <c r="G28" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="H28" s="24" t="s">
+      <c r="H28" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="I28" s="49" t="s">
+      <c r="I28" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="50" t="s">
+      <c r="J28" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="K28" s="50" t="s">
+      <c r="K28" s="52" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="29" spans="4:11">
+      <c r="L28" s="52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="4:12">
       <c r="D29" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="E29" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="43"/>
-      <c r="G29" s="26"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="G29" s="43"/>
       <c r="H29" s="26"/>
-      <c r="I29" s="51" t="s">
-        <v>37</v>
-      </c>
-      <c r="J29" s="26"/>
-      <c r="K29" s="52"/>
-    </row>
-    <row r="30" spans="4:11">
+      <c r="I29" s="26"/>
+      <c r="J29" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="K29" s="26"/>
+      <c r="L29" s="54"/>
+    </row>
+    <row r="30" spans="4:12">
       <c r="D30" s="26"/>
-      <c r="E30" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" s="43"/>
-      <c r="G30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="43"/>
       <c r="H30" s="26"/>
-      <c r="I30" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="J30" s="26"/>
-      <c r="K30" s="52"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" s="26"/>
+      <c r="L30" s="54"/>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="28" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B36" s="28"/>
       <c r="C36" s="28"/>
       <c r="D36" s="28"/>
-      <c r="E36" s="45"/>
-    </row>
-    <row r="37" ht="15.75" spans="1:7">
+      <c r="E36" s="28"/>
+      <c r="F36" s="45"/>
+    </row>
+    <row r="37" ht="15.75" spans="1:8">
       <c r="A37" s="29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B37" s="29"/>
       <c r="C37" s="29"/>
       <c r="D37" s="29"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="46"/>
       <c r="G37" s="29"/>
-    </row>
-    <row r="38" ht="15.75" spans="1:7">
+      <c r="H37" s="29"/>
+    </row>
+    <row r="38" ht="15.75" spans="1:8">
       <c r="A38" s="29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B38" s="29"/>
       <c r="C38" s="29"/>
       <c r="D38" s="29"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="46"/>
       <c r="G38" s="29"/>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="H38" s="29"/>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B39" s="31"/>
       <c r="C39" s="31"/>
       <c r="D39" s="31"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="47"/>
       <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A39:G39"/>
+  <mergeCells count="19">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="A39:H39"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
@@ -2577,11 +2644,12 @@
     <mergeCell ref="D29:D30"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
-    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="G5:G6"/>
     <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J29:J30"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="K29:K30"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L29:L30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2606,7 +2674,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2650,7 +2718,7 @@
     </row>
     <row r="3" ht="23.25" spans="1:19">
       <c r="A3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2673,11 +2741,11 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -2688,33 +2756,33 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" ht="28.5" customHeight="1" spans="1:19">
       <c r="A6" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2739,16 +2807,16 @@
         <v>0.01</v>
       </c>
       <c r="P6" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q6" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R6" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S6" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -2776,16 +2844,16 @@
         <v>0.01</v>
       </c>
       <c r="P7" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q7" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R7" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S7" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -2813,16 +2881,16 @@
         <v>0.01</v>
       </c>
       <c r="P8" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q8" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R8" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S8" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -2850,22 +2918,22 @@
         <v>0.01</v>
       </c>
       <c r="P9" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q9" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R9" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S9" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1" spans="1:19">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
@@ -2889,21 +2957,21 @@
         <v>0.01</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q10" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="R10" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="S10" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2928,21 +2996,21 @@
         <v>0.05</v>
       </c>
       <c r="P11" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q11" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R11" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S11" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -2967,16 +3035,16 @@
         <v>0.95</v>
       </c>
       <c r="P12" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q12" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R12" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S12" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>